<commit_message>
githubScaping topics in json
</commit_message>
<xml_diff>
--- a/web_scrapping/BatsmenDetail.xlsx
+++ b/web_scrapping/BatsmenDetail.xlsx
@@ -410,39 +410,39 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>KL Rahul (c)†</v>
+        <v>Virat Kohli (c)</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>535</v>
+        <v>405</v>
       </c>
       <c r="D2">
-        <v>394</v>
+        <v>339</v>
       </c>
       <c r="E2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F2">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve">Mayank Agarwal </v>
+        <v xml:space="preserve">Devdutt Padikkal </v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>342</v>
+        <v>411</v>
       </c>
       <c r="D3">
-        <v>256</v>
+        <v>328</v>
       </c>
       <c r="E3">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F3">
         <v>14</v>
@@ -450,279 +450,279 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v xml:space="preserve">Chris Gayle </v>
+        <v xml:space="preserve">Rajat Patidar </v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="D4">
-        <v>154</v>
+        <v>62</v>
       </c>
       <c r="E4">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v xml:space="preserve">Deepak Hooda </v>
+        <v xml:space="preserve">Glenn Maxwell </v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>160</v>
+        <v>513</v>
       </c>
       <c r="D5">
-        <v>123</v>
+        <v>356</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v xml:space="preserve">Nicholas Pooran </v>
+        <v>AB de Villiers †</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>85</v>
+        <v>207</v>
       </c>
       <c r="D6">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v xml:space="preserve">M Shahrukh Khan </v>
+        <v xml:space="preserve">Washington Sundar </v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>153</v>
+        <v>31</v>
       </c>
       <c r="D7">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v xml:space="preserve">Prithvi Shaw </v>
+        <v xml:space="preserve">Daniel Sams </v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>479</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>301</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v xml:space="preserve">Shikhar Dhawan </v>
+        <v xml:space="preserve">Prithvi Shaw </v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>587</v>
+        <v>479</v>
       </c>
       <c r="D9">
-        <v>471</v>
+        <v>301</v>
       </c>
       <c r="E9">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F9">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v xml:space="preserve">Steven Smith </v>
+        <v xml:space="preserve">Shikhar Dhawan </v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>152</v>
+        <v>587</v>
       </c>
       <c r="D10">
-        <v>135</v>
+        <v>471</v>
       </c>
       <c r="E10">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Rishabh Pant (c)†</v>
+        <v xml:space="preserve">Steven Smith </v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>419</v>
+        <v>152</v>
       </c>
       <c r="D11">
-        <v>326</v>
+        <v>135</v>
       </c>
       <c r="E11">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v xml:space="preserve">Marcus Stoinis </v>
+        <v>Rishabh Pant (c)†</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>89</v>
+        <v>419</v>
       </c>
       <c r="D12">
-        <v>72</v>
+        <v>326</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v xml:space="preserve">Lalit Yadav </v>
+        <v xml:space="preserve">Marcus Stoinis </v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="D13">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v xml:space="preserve">Shreyas Iyer </v>
+        <v xml:space="preserve">Shimron Hetmyer </v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>175</v>
+        <v>242</v>
       </c>
       <c r="D14">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v xml:space="preserve">Axar Patel </v>
+        <v>Srikar Bharat †</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15">
-        <v>40</v>
+        <v>191</v>
       </c>
       <c r="D15">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v xml:space="preserve">Shimron Hetmyer </v>
+        <v xml:space="preserve">AB de Villiers </v>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C16">
-        <v>242</v>
+        <v>106</v>
       </c>
       <c r="D16">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F16">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v xml:space="preserve">Tom Curran </v>
+        <v xml:space="preserve">Dan Christian </v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D17">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -730,239 +730,239 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v xml:space="preserve">Ruturaj Gaikwad </v>
+        <v xml:space="preserve">Shahbaz Ahmed </v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>635</v>
+        <v>59</v>
       </c>
       <c r="D18">
-        <v>466</v>
+        <v>53</v>
       </c>
       <c r="E18">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="F18">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v xml:space="preserve">Faf du Plessis </v>
+        <v xml:space="preserve">Kyle Jamieson </v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>633</v>
+        <v>65</v>
       </c>
       <c r="D19">
-        <v>458</v>
+        <v>55</v>
       </c>
       <c r="E19">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v xml:space="preserve">Robin Uthappa </v>
+        <v>Rohit Sharma (c)</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C20">
-        <v>115</v>
+        <v>381</v>
       </c>
       <c r="D20">
-        <v>84</v>
+        <v>299</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v xml:space="preserve">Shardul Thakur </v>
+        <v>Quinton de Kock †</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>297</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>256</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v xml:space="preserve">Ambati Rayudu </v>
+        <v xml:space="preserve">Ishan Kishan </v>
       </c>
       <c r="B22">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>257</v>
+        <v>79</v>
       </c>
       <c r="D22">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="E22">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F22">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v xml:space="preserve">Moeen Ali </v>
+        <v xml:space="preserve">Suryakumar Yadav </v>
       </c>
       <c r="B23">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23">
-        <v>357</v>
+        <v>317</v>
       </c>
       <c r="D23">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="E23">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F23">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>MS Dhoni (c)†</v>
+        <v xml:space="preserve">Krunal Pandya </v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="D24">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="E24">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v xml:space="preserve">Ravindra Jadeja </v>
+        <v xml:space="preserve">Kieron Pollard </v>
       </c>
       <c r="B25">
         <v>12</v>
       </c>
       <c r="C25">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D25">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E25">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F25">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v xml:space="preserve">Aiden Markram </v>
+        <v xml:space="preserve">Hardik Pandya </v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="D26">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E26">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v xml:space="preserve">Harpreet Brar </v>
+        <v xml:space="preserve">Adam Milne </v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="D27">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="E27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v xml:space="preserve">Nathan Ellis </v>
+        <v xml:space="preserve">Rahul Chahar </v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v xml:space="preserve">Mohammed Shami </v>
+        <v xml:space="preserve">Jasprit Bumrah </v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C29">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>17</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -970,16 +970,16 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v xml:space="preserve">David Warner </v>
+        <v xml:space="preserve">Trent Boult </v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -990,16 +990,16 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Wriddhiman Saha †</v>
+        <v>KL Rahul (c)</v>
       </c>
       <c r="B31">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="D31">
-        <v>140</v>
+        <v>57</v>
       </c>
       <c r="E31">
         <v>7</v>
@@ -1010,19 +1010,19 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Kane Williamson (c)</v>
+        <v>Prabhsimran Singh †</v>
       </c>
       <c r="B32">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C32">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="D32">
-        <v>155</v>
+        <v>23</v>
       </c>
       <c r="E32">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1030,19 +1030,19 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v xml:space="preserve">Manish Pandey </v>
+        <v xml:space="preserve">Chris Gayle </v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C33">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="D33">
-        <v>195</v>
+        <v>154</v>
       </c>
       <c r="E33">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F33">
         <v>8</v>
@@ -1050,79 +1050,79 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v xml:space="preserve">Kedar Jadhav </v>
+        <v xml:space="preserve">Nicholas Pooran </v>
       </c>
       <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>85</v>
+      </c>
+      <c r="D34">
+        <v>76</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
         <v>5</v>
-      </c>
-      <c r="C34">
-        <v>55</v>
-      </c>
-      <c r="D34">
-        <v>52</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="F34">
-        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v xml:space="preserve">Abdul Samad </v>
+        <v xml:space="preserve">Deepak Hooda </v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="D35">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F35">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v xml:space="preserve">Jason Holder </v>
+        <v xml:space="preserve">M Shahrukh Khan </v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C36">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D36">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F36">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v xml:space="preserve">Rashid Khan </v>
+        <v xml:space="preserve">Harpreet Brar </v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C37">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="D37">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E37">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F37">
         <v>2</v>
@@ -1130,559 +1130,559 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v xml:space="preserve">Bhuvneshwar Kumar </v>
+        <v xml:space="preserve">Harshal Patel </v>
       </c>
       <c r="B38">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D38">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v xml:space="preserve">Nitish Rana </v>
+        <v xml:space="preserve">Mohammed Siraj </v>
       </c>
       <c r="B39">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C39">
-        <v>383</v>
+        <v>20</v>
       </c>
       <c r="D39">
-        <v>314</v>
+        <v>26</v>
       </c>
       <c r="E39">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="F39">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v xml:space="preserve">Shubman Gill </v>
+        <v xml:space="preserve">Ruturaj Gaikwad </v>
       </c>
       <c r="B40">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40">
-        <v>478</v>
+        <v>635</v>
       </c>
       <c r="D40">
-        <v>402</v>
+        <v>466</v>
       </c>
       <c r="E40">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="F40">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v xml:space="preserve">Rahul Tripathi </v>
+        <v xml:space="preserve">Faf du Plessis </v>
       </c>
       <c r="B41">
         <v>16</v>
       </c>
       <c r="C41">
-        <v>397</v>
+        <v>633</v>
       </c>
       <c r="D41">
-        <v>283</v>
+        <v>458</v>
       </c>
       <c r="E41">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="F41">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v xml:space="preserve">Andre Russell </v>
+        <v xml:space="preserve">Moeen Ali </v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C42">
-        <v>183</v>
+        <v>357</v>
       </c>
       <c r="D42">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="E42">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F42">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Eoin Morgan (c)</v>
+        <v xml:space="preserve">Ambati Rayudu </v>
       </c>
       <c r="B43">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>257</v>
+      </c>
+      <c r="D43">
+        <v>170</v>
+      </c>
+      <c r="E43">
         <v>16</v>
       </c>
-      <c r="C43">
-        <v>133</v>
-      </c>
-      <c r="D43">
-        <v>139</v>
-      </c>
-      <c r="E43">
-        <v>8</v>
-      </c>
       <c r="F43">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Dinesh Karthik †</v>
+        <v xml:space="preserve">Suresh Raina </v>
       </c>
       <c r="B44">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C44">
-        <v>223</v>
+        <v>160</v>
       </c>
       <c r="D44">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="E44">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F44">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v xml:space="preserve">Shakib Al Hasan </v>
+        <v>MS Dhoni (c)†</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C45">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="D45">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="E45">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>David Warner (c)</v>
+        <v xml:space="preserve">Ravindra Jadeja </v>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C46">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="D46">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E46">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F46">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v xml:space="preserve">Jonny Bairstow </v>
+        <v xml:space="preserve">Dwayne Bravo </v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D47">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="E47">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F47">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v xml:space="preserve">Mohammad Nabi </v>
+        <v xml:space="preserve">Shardul Thakur </v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C48">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="D48">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E48">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v xml:space="preserve">Vijay Shankar </v>
+        <v xml:space="preserve">Anmolpreet Singh </v>
       </c>
       <c r="B49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="D49">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F49">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v xml:space="preserve">Suresh Raina </v>
+        <v xml:space="preserve">Saurabh Tiwary </v>
       </c>
       <c r="B50">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C50">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="D50">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="E50">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F50">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v xml:space="preserve">Evin Lewis </v>
+        <v>Kieron Pollard (c)</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>151</v>
+        <v>15</v>
       </c>
       <c r="D51">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="E51">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F51">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v xml:space="preserve">Yashasvi Jaiswal </v>
+        <v xml:space="preserve">Shreyas Iyer </v>
       </c>
       <c r="B52">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C52">
-        <v>249</v>
+        <v>175</v>
       </c>
       <c r="D52">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E52">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="F52">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Sanju Samson (c)†</v>
+        <v xml:space="preserve">Axar Patel </v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C53">
-        <v>484</v>
+        <v>40</v>
       </c>
       <c r="D53">
-        <v>354</v>
+        <v>46</v>
       </c>
       <c r="E53">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="F53">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v xml:space="preserve">Shivam Dube </v>
+        <v xml:space="preserve">Shubman Gill </v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C54">
-        <v>230</v>
+        <v>478</v>
       </c>
       <c r="D54">
-        <v>193</v>
+        <v>402</v>
       </c>
       <c r="E54">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F54">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v xml:space="preserve">Glenn Phillips </v>
+        <v xml:space="preserve">Venkatesh Iyer </v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C55">
-        <v>26</v>
+        <v>370</v>
       </c>
       <c r="D55">
-        <v>33</v>
+        <v>288</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="F55">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>Virat Kohli (c)</v>
+        <v xml:space="preserve">Nitish Rana </v>
       </c>
       <c r="B56">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>405</v>
+        <v>383</v>
       </c>
       <c r="D56">
-        <v>339</v>
+        <v>314</v>
       </c>
       <c r="E56">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F56">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v xml:space="preserve">Devdutt Padikkal </v>
+        <v xml:space="preserve">Rahul Tripathi </v>
       </c>
       <c r="B57">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C57">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="D57">
-        <v>328</v>
+        <v>283</v>
       </c>
       <c r="E57">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F57">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v xml:space="preserve">AB de Villiers </v>
+        <v>Dinesh Karthik †</v>
       </c>
       <c r="B58">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C58">
-        <v>106</v>
+        <v>223</v>
       </c>
       <c r="D58">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="E58">
+        <v>22</v>
+      </c>
+      <c r="F58">
         <v>7</v>
-      </c>
-      <c r="F58">
-        <v>6</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v xml:space="preserve">Glenn Maxwell </v>
+        <v>Eoin Morgan (c)</v>
       </c>
       <c r="B59">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C59">
-        <v>513</v>
+        <v>133</v>
       </c>
       <c r="D59">
-        <v>356</v>
+        <v>139</v>
       </c>
       <c r="E59">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F59">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v xml:space="preserve">Tim David </v>
+        <v xml:space="preserve">Shakib Al Hasan </v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D60">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v xml:space="preserve">Harshal Patel </v>
+        <v xml:space="preserve">Sunil Narine </v>
       </c>
       <c r="B61">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C61">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D61">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E61">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F61">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v xml:space="preserve">Wanindu Hasaranga de Silva </v>
+        <v xml:space="preserve">Lockie Ferguson </v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v xml:space="preserve">Ajinkya Rahane </v>
+        <v>David Warner (c)</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C63">
-        <v>8</v>
+        <v>193</v>
       </c>
       <c r="D63">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v xml:space="preserve">Chris Woakes </v>
+        <v>Jonny Bairstow †</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C64">
-        <v>15</v>
+        <v>181</v>
       </c>
       <c r="D64">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v xml:space="preserve">Ravichandran Ashwin </v>
+        <v xml:space="preserve">Kane Williamson </v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C65">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="D65">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="E65">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -1690,19 +1690,19 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v xml:space="preserve">Kagiso Rabada </v>
+        <v xml:space="preserve">Virat Singh </v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D66">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -1710,179 +1710,179 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v xml:space="preserve">Jos Buttler </v>
+        <v xml:space="preserve">Kedar Jadhav </v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C67">
-        <v>254</v>
+        <v>55</v>
       </c>
       <c r="D67">
-        <v>166</v>
+        <v>52</v>
       </c>
       <c r="E67">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="F67">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v xml:space="preserve">Manan Vohra </v>
+        <v xml:space="preserve">Abhishek Sharma </v>
       </c>
       <c r="B68">
+        <v>7</v>
+      </c>
+      <c r="C68">
+        <v>98</v>
+      </c>
+      <c r="D68">
+        <v>75</v>
+      </c>
+      <c r="E68">
+        <v>7</v>
+      </c>
+      <c r="F68">
         <v>4</v>
-      </c>
-      <c r="C68">
-        <v>42</v>
-      </c>
-      <c r="D68">
-        <v>39</v>
-      </c>
-      <c r="E68">
-        <v>5</v>
-      </c>
-      <c r="F68">
-        <v>2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v xml:space="preserve">David Miller </v>
+        <v xml:space="preserve">Rashid Khan </v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C69">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="D69">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="E69">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F69">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v xml:space="preserve">Riyan Parag </v>
+        <v xml:space="preserve">Vijay Shankar </v>
       </c>
       <c r="B70">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C70">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="D70">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E70">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F70">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v xml:space="preserve">Rahul Tewatia </v>
+        <v xml:space="preserve">Jagadeesha Suchith </v>
       </c>
       <c r="B71">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C71">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="D71">
-        <v>147</v>
+        <v>6</v>
       </c>
       <c r="E71">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F71">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v xml:space="preserve">Chris Morris </v>
+        <v xml:space="preserve">Andre Russell </v>
       </c>
       <c r="B72">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C72">
-        <v>67</v>
+        <v>183</v>
       </c>
       <c r="D72">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="E72">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F72">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v xml:space="preserve">Jaydev Unadkat </v>
+        <v xml:space="preserve">Pat Cummins </v>
       </c>
       <c r="B73">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C73">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="D73">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E73">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F73">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v xml:space="preserve">Jhye Richardson </v>
+        <v xml:space="preserve">Shivam Mavi </v>
       </c>
       <c r="B74">
         <v>2</v>
       </c>
       <c r="C74">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D74">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E74">
         <v>2</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v xml:space="preserve">Murugan Ashwin </v>
+        <v xml:space="preserve">Prasidh Krishna </v>
       </c>
       <c r="B75">
         <v>2</v>
       </c>
       <c r="C75">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -1890,233 +1890,233 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v xml:space="preserve">Riley Meredith </v>
+        <v xml:space="preserve">Jos Buttler </v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>254</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v xml:space="preserve">Sam Curran </v>
+        <v xml:space="preserve">Yashasvi Jaiswal </v>
       </c>
       <c r="B77">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C77">
-        <v>56</v>
+        <v>249</v>
       </c>
       <c r="D77">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="E77">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F77">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v xml:space="preserve">Sunil Narine </v>
+        <v>Sanju Samson (c)†</v>
       </c>
       <c r="B78">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C78">
-        <v>62</v>
+        <v>484</v>
       </c>
       <c r="D78">
-        <v>47</v>
+        <v>354</v>
       </c>
       <c r="E78">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="F78">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v xml:space="preserve">Pat Cummins </v>
+        <v xml:space="preserve">Shivam Dube </v>
       </c>
       <c r="B79">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C79">
-        <v>93</v>
+        <v>230</v>
       </c>
       <c r="D79">
-        <v>56</v>
+        <v>193</v>
       </c>
       <c r="E79">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F79">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>Rohit Sharma (c)</v>
+        <v xml:space="preserve">Rahul Tewatia </v>
       </c>
       <c r="B80">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C80">
-        <v>381</v>
+        <v>155</v>
       </c>
       <c r="D80">
-        <v>299</v>
+        <v>147</v>
       </c>
       <c r="E80">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="F80">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>Quinton de Kock †</v>
+        <v xml:space="preserve">David Miller </v>
       </c>
       <c r="B81">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>124</v>
+      </c>
+      <c r="D81">
+        <v>113</v>
+      </c>
+      <c r="E81">
         <v>11</v>
       </c>
-      <c r="C81">
-        <v>297</v>
-      </c>
-      <c r="D81">
-        <v>256</v>
-      </c>
-      <c r="E81">
-        <v>29</v>
-      </c>
       <c r="F81">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v xml:space="preserve">Suryakumar Yadav </v>
+        <v>KL Rahul (c)†</v>
       </c>
       <c r="B82">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C82">
-        <v>317</v>
+        <v>535</v>
       </c>
       <c r="D82">
-        <v>221</v>
+        <v>394</v>
       </c>
       <c r="E82">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F82">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v xml:space="preserve">Ishan Kishan </v>
+        <v xml:space="preserve">Mayank Agarwal </v>
       </c>
       <c r="B83">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C83">
-        <v>79</v>
+        <v>342</v>
       </c>
       <c r="D83">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="E83">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="F83">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v xml:space="preserve">Kieron Pollard </v>
+        <v xml:space="preserve">Moises Henriques </v>
       </c>
       <c r="B84">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C84">
-        <v>230</v>
+        <v>31</v>
       </c>
       <c r="D84">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="E84">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v xml:space="preserve">Krunal Pandya </v>
+        <v xml:space="preserve">Chris Jordan </v>
       </c>
       <c r="B85">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C85">
-        <v>143</v>
+        <v>32</v>
       </c>
       <c r="D85">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="E85">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F85">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v xml:space="preserve">Saurabh Tiwary </v>
+        <v xml:space="preserve">Ravi Bishnoi </v>
       </c>
       <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
         <v>4</v>
       </c>
-      <c r="C86">
-        <v>115</v>
-      </c>
-      <c r="D86">
-        <v>97</v>
-      </c>
       <c r="E86">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v xml:space="preserve">Adam Milne </v>
+        <v xml:space="preserve">Mohammed Shami </v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C87">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D87">
         <v>17</v>
@@ -2125,44 +2125,44 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v xml:space="preserve">Venkatesh Iyer </v>
+        <v xml:space="preserve">Arshdeep Singh </v>
       </c>
       <c r="B88">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C88">
-        <v>370</v>
+        <v>2</v>
       </c>
       <c r="D88">
-        <v>288</v>
+        <v>3</v>
       </c>
       <c r="E88">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v xml:space="preserve">Mandeep Singh </v>
+        <v xml:space="preserve">George Garton </v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C89">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D89">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E89">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -2170,99 +2170,99 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v xml:space="preserve">Hardik Pandya </v>
+        <v xml:space="preserve">Aiden Markram </v>
       </c>
       <c r="B90">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C90">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="D90">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E90">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F90">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v xml:space="preserve">Shivam Mavi </v>
+        <v xml:space="preserve">Sarfaraz Khan </v>
       </c>
       <c r="B91">
         <v>2</v>
       </c>
       <c r="C91">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E91">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v xml:space="preserve">Prasidh Krishna </v>
+        <v xml:space="preserve">Robin Uthappa </v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>Jonny Bairstow †</v>
+        <v xml:space="preserve">Varun Chakravarthy </v>
       </c>
       <c r="B93">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C93">
-        <v>181</v>
+        <v>2</v>
       </c>
       <c r="D93">
-        <v>122</v>
+        <v>4</v>
       </c>
       <c r="E93">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v xml:space="preserve">Kane Williamson </v>
+        <v xml:space="preserve">Nathan Ellis </v>
       </c>
       <c r="B94">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="D94">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="E94">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -2270,19 +2270,19 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v xml:space="preserve">Virat Singh </v>
+        <v xml:space="preserve">David Warner </v>
       </c>
       <c r="B95">
         <v>2</v>
       </c>
       <c r="C95">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D95">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95">
         <v>0</v>
@@ -2290,39 +2290,39 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v xml:space="preserve">Abhishek Sharma </v>
+        <v>Wriddhiman Saha †</v>
       </c>
       <c r="B96">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C96">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="D96">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="E96">
         <v>7</v>
       </c>
       <c r="F96">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v xml:space="preserve">Jagadeesha Suchith </v>
+        <v>Kane Williamson (c)</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C97">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="D97">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="E97">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -2330,79 +2330,79 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v xml:space="preserve">Jayant Yadav </v>
+        <v xml:space="preserve">Manish Pandey </v>
       </c>
       <c r="B98">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C98">
-        <v>34</v>
+        <v>223</v>
       </c>
       <c r="D98">
-        <v>26</v>
+        <v>195</v>
       </c>
       <c r="E98">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F98">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v xml:space="preserve">Rahul Chahar </v>
+        <v xml:space="preserve">Abdul Samad </v>
       </c>
       <c r="B99">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C99">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="D99">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v xml:space="preserve">Jasprit Bumrah </v>
+        <v xml:space="preserve">Jason Holder </v>
       </c>
       <c r="B100">
         <v>7</v>
       </c>
       <c r="C100">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="D100">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="E100">
         <v>2</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v xml:space="preserve">Trent Boult </v>
+        <v xml:space="preserve">Bhuvneshwar Kumar </v>
       </c>
       <c r="B101">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D101">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -2410,99 +2410,99 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v xml:space="preserve">Lockie Ferguson </v>
+        <v>Mayank Agarwal (c)</v>
       </c>
       <c r="B102">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C102">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="D102">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F102">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v xml:space="preserve">Varun Chakravarthy </v>
+        <v xml:space="preserve">Dawid Malan </v>
       </c>
       <c r="B103">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C103">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D103">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v xml:space="preserve">Mahipal Lomror </v>
+        <v xml:space="preserve">Tim Seifert </v>
       </c>
       <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
+      </c>
+      <c r="D104">
         <v>4</v>
       </c>
-      <c r="C104">
-        <v>94</v>
-      </c>
-      <c r="D104">
-        <v>73</v>
-      </c>
       <c r="E104">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F104">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v xml:space="preserve">Liam Livingstone </v>
+        <v xml:space="preserve">Fabian Allen </v>
       </c>
       <c r="B105">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C105">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D105">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E105">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v xml:space="preserve">Chetan Sakariya </v>
+        <v xml:space="preserve">Nathan Coulter-Nile </v>
       </c>
       <c r="B106">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C106">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D106">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E106">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F106">
         <v>0</v>
@@ -2510,99 +2510,99 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v xml:space="preserve">Kartik Tyagi </v>
+        <v xml:space="preserve">Jayant Yadav </v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D107">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>Srikar Bharat †</v>
+        <v xml:space="preserve">Ravichandran Ashwin </v>
       </c>
       <c r="B108">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C108">
-        <v>191</v>
+        <v>44</v>
       </c>
       <c r="D108">
-        <v>156</v>
+        <v>42</v>
       </c>
       <c r="E108">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F108">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v xml:space="preserve">Chris Lynn </v>
+        <v xml:space="preserve">Mujeeb Ur Rahman </v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="D109">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E109">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>Ishan Kishan †</v>
+        <v xml:space="preserve">Khaleel Ahmed </v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C110">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D110">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="E110">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F110">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v xml:space="preserve">Marco Jansen </v>
+        <v xml:space="preserve">Ripal Patel </v>
       </c>
       <c r="B111">
         <v>2</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D111">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -2610,39 +2610,39 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v xml:space="preserve">Washington Sundar </v>
+        <v xml:space="preserve">Jason Roy </v>
       </c>
       <c r="B112">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C112">
-        <v>31</v>
+        <v>150</v>
       </c>
       <c r="D112">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="E112">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v xml:space="preserve">Rajat Patidar </v>
+        <v xml:space="preserve">Priyam Garg </v>
       </c>
       <c r="B113">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C113">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D113">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E113">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F113">
         <v>3</v>
@@ -2650,59 +2650,59 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>AB de Villiers †</v>
+        <v>Ishan Kishan †</v>
       </c>
       <c r="B114">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C114">
-        <v>207</v>
+        <v>162</v>
       </c>
       <c r="D114">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="E114">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F114">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v xml:space="preserve">Shahbaz Ahmed </v>
+        <v xml:space="preserve">James Neesham </v>
       </c>
       <c r="B115">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C115">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="E115">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F115">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v xml:space="preserve">Dan Christian </v>
+        <v xml:space="preserve">Piyush Chawla </v>
       </c>
       <c r="B116">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C116">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -2710,59 +2710,59 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v xml:space="preserve">Kyle Jamieson </v>
+        <v>Manish Pandey (c)</v>
       </c>
       <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117">
+        <v>69</v>
+      </c>
+      <c r="D117">
+        <v>41</v>
+      </c>
+      <c r="E117">
         <v>7</v>
       </c>
-      <c r="C117">
-        <v>65</v>
-      </c>
-      <c r="D117">
-        <v>55</v>
-      </c>
-      <c r="E117">
-        <v>5</v>
-      </c>
       <c r="F117">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v xml:space="preserve">Mohammed Siraj </v>
+        <v xml:space="preserve">Mohammad Nabi </v>
       </c>
       <c r="B118">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C118">
+        <v>34</v>
+      </c>
+      <c r="D118">
         <v>20</v>
       </c>
-      <c r="D118">
-        <v>26</v>
-      </c>
       <c r="E118">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F118">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v xml:space="preserve">Harbhajan Singh </v>
+        <v xml:space="preserve">Siddarth Kaul </v>
       </c>
       <c r="B119">
         <v>2</v>
       </c>
       <c r="C119">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D119">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -2770,159 +2770,159 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v xml:space="preserve">Avesh Khan </v>
+        <v xml:space="preserve">Evin Lewis </v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C120">
-        <v>5</v>
+        <v>151</v>
       </c>
       <c r="D120">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v xml:space="preserve">Tim Southee </v>
+        <v xml:space="preserve">Liam Livingstone </v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C121">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D121">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v xml:space="preserve">Tim Seifert </v>
+        <v xml:space="preserve">Mahipal Lomror </v>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="D122">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v xml:space="preserve">Fabian Allen </v>
+        <v xml:space="preserve">Riyan Parag </v>
       </c>
       <c r="B123">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C123">
+        <v>93</v>
+      </c>
+      <c r="D123">
+        <v>83</v>
+      </c>
+      <c r="E123">
         <v>6</v>
       </c>
-      <c r="D123">
-        <v>12</v>
-      </c>
-      <c r="E123">
-        <v>0</v>
-      </c>
       <c r="F123">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v xml:space="preserve">Ben Stokes </v>
+        <v xml:space="preserve">Chris Lynn </v>
       </c>
       <c r="B124">
         <v>1</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="D124">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v xml:space="preserve">Mustafizur Rahman </v>
+        <v xml:space="preserve">Marco Jansen </v>
       </c>
       <c r="B125">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C125">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D125">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E125">
         <v>0</v>
       </c>
       <c r="F125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v xml:space="preserve">Ripal Patel </v>
+        <v xml:space="preserve">Chris Morris </v>
       </c>
       <c r="B126">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C126">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D126">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E126">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F126">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v xml:space="preserve">Sandeep Sharma </v>
+        <v xml:space="preserve">Chetan Sakariya </v>
       </c>
       <c r="B127">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C127">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D127">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F127">
         <v>0</v>
@@ -2930,16 +2930,16 @@
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v xml:space="preserve">Nathan Coulter-Nile </v>
+        <v xml:space="preserve">Kartik Tyagi </v>
       </c>
       <c r="B128">
         <v>2</v>
       </c>
       <c r="C128">
+        <v>2</v>
+      </c>
+      <c r="D128">
         <v>4</v>
-      </c>
-      <c r="D128">
-        <v>5</v>
       </c>
       <c r="E128">
         <v>0</v>
@@ -2950,67 +2950,67 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v xml:space="preserve">Jason Roy </v>
+        <v xml:space="preserve">Mandeep Singh </v>
       </c>
       <c r="B129">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C129">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="D129">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="E129">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F129">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v xml:space="preserve">Priyam Garg </v>
+        <v xml:space="preserve">Navdeep Saini </v>
       </c>
       <c r="B130">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C130">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="D130">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="E130">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F130">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v xml:space="preserve">Shreyas Gopal </v>
+        <v xml:space="preserve">Yuzvendra Chahal </v>
       </c>
       <c r="B131">
         <v>2</v>
       </c>
       <c r="C131">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D131">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E131">
         <v>0</v>
       </c>
       <c r="F131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v xml:space="preserve">Kuldip Yadav </v>
+        <v xml:space="preserve">Dhawal Kulkarni </v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="D132">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E132">
         <v>0</v>
@@ -3030,73 +3030,73 @@
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v xml:space="preserve">George Garton </v>
+        <v xml:space="preserve">Sam Curran </v>
       </c>
       <c r="B133">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C133">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D133">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v xml:space="preserve">Sarfaraz Khan </v>
+        <v xml:space="preserve">Mustafizur Rahman </v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D134">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E134">
         <v>0</v>
       </c>
       <c r="F134">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v xml:space="preserve">Moises Henriques </v>
+        <v xml:space="preserve">Sachin Baby </v>
       </c>
       <c r="B135">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C135">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D135">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E135">
         <v>0</v>
       </c>
       <c r="F135">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v xml:space="preserve">Kamlesh Nagarkoti </v>
+        <v xml:space="preserve">Wanindu Hasaranga de Silva </v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D136">
         <v>2</v>
@@ -3110,19 +3110,19 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v xml:space="preserve">Sachin Baby </v>
+        <v xml:space="preserve">Tom Curran </v>
       </c>
       <c r="B137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C137">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D137">
         <v>17</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F137">
         <v>0</v>
@@ -3130,19 +3130,19 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v xml:space="preserve">Yuzvendra Chahal </v>
+        <v xml:space="preserve">Jhye Richardson </v>
       </c>
       <c r="B138">
         <v>2</v>
       </c>
       <c r="C138">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D138">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F138">
         <v>0</v>
@@ -3150,16 +3150,16 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v xml:space="preserve">Siddarth Kaul </v>
+        <v xml:space="preserve">Murugan Ashwin </v>
       </c>
       <c r="B139">
         <v>2</v>
       </c>
       <c r="C139">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D139">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E139">
         <v>1</v>
@@ -3170,39 +3170,39 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v xml:space="preserve">Dwayne Bravo </v>
+        <v xml:space="preserve">Riley Meredith </v>
       </c>
       <c r="B140">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C140">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="D140">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E140">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F140">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v xml:space="preserve">Daniel Sams </v>
+        <v xml:space="preserve">Kagiso Rabada </v>
       </c>
       <c r="B141">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C141">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D141">
         <v>6</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F141">
         <v>0</v>
@@ -3210,67 +3210,67 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v xml:space="preserve">James Neesham </v>
+        <v xml:space="preserve">Glenn Phillips </v>
       </c>
       <c r="B142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D142">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="E142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F142">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v xml:space="preserve">Piyush Chawla </v>
+        <v xml:space="preserve">Shreyas Gopal </v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D143">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E143">
         <v>0</v>
       </c>
       <c r="F143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>Manish Pandey (c)</v>
+        <v xml:space="preserve">Kuldip Yadav </v>
       </c>
       <c r="B144">
         <v>1</v>
       </c>
       <c r="C144">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="D144">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="E144">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F144">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v xml:space="preserve">Mujeeb Ur Rahman </v>
+        <v xml:space="preserve">Tim David </v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -3279,7 +3279,7 @@
         <v>1</v>
       </c>
       <c r="D145">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E145">
         <v>0</v>
@@ -3290,13 +3290,13 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v xml:space="preserve">Khaleel Ahmed </v>
+        <v xml:space="preserve">Kamlesh Nagarkoti </v>
       </c>
       <c r="B146">
         <v>1</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D146">
         <v>2</v>
@@ -3310,13 +3310,13 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v xml:space="preserve">Navdeep Saini </v>
+        <v xml:space="preserve">Harbhajan Singh </v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C147">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D147">
         <v>4</v>
@@ -3330,19 +3330,19 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v xml:space="preserve">Tabraiz Shamsi </v>
+        <v xml:space="preserve">Lalit Yadav </v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C148">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D148">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F148">
         <v>0</v>
@@ -3350,147 +3350,147 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v xml:space="preserve">Anmolpreet Singh </v>
+        <v xml:space="preserve">Avesh Khan </v>
       </c>
       <c r="B149">
         <v>1</v>
       </c>
       <c r="C149">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D149">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F149">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>Kieron Pollard (c)</v>
+        <v xml:space="preserve">Tim Southee </v>
       </c>
       <c r="B150">
         <v>1</v>
       </c>
       <c r="C150">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D150">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F150">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>Prabhsimran Singh †</v>
+        <v xml:space="preserve">Jonny Bairstow </v>
       </c>
       <c r="B151">
         <v>2</v>
       </c>
       <c r="C151">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="D151">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="E151">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F151">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>Mayank Agarwal (c)</v>
+        <v xml:space="preserve">Manan Vohra </v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C152">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="D152">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="E152">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F152">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v xml:space="preserve">Dawid Malan </v>
+        <v xml:space="preserve">Ajinkya Rahane </v>
       </c>
       <c r="B153">
         <v>1</v>
       </c>
       <c r="C153">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D153">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E153">
         <v>1</v>
       </c>
       <c r="F153">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v xml:space="preserve">Chris Jordan </v>
+        <v xml:space="preserve">Chris Woakes </v>
       </c>
       <c r="B154">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C154">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D154">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F154">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v xml:space="preserve">Shahbaz Nadeem </v>
+        <v xml:space="preserve">Jaydev Unadkat </v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D155">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E155">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F155">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v xml:space="preserve">T Natarajan </v>
+        <v xml:space="preserve">Anuj Rawat </v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -3499,7 +3499,7 @@
         <v>0</v>
       </c>
       <c r="D156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E156">
         <v>0</v>
@@ -3510,39 +3510,39 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>KL Rahul (c)</v>
+        <v xml:space="preserve">Deepak Chahar </v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C157">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="D157">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E157">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F157">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v xml:space="preserve">Arshdeep Singh </v>
+        <v xml:space="preserve">Sandeep Sharma </v>
       </c>
       <c r="B158">
         <v>2</v>
       </c>
       <c r="C158">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D158">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F158">
         <v>0</v>
@@ -3550,16 +3550,16 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v xml:space="preserve">Ravi Bishnoi </v>
+        <v xml:space="preserve">Shahbaz Nadeem </v>
       </c>
       <c r="B159">
         <v>1</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D159">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E159">
         <v>0</v>
@@ -3570,16 +3570,16 @@
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v xml:space="preserve">Deepak Chahar </v>
+        <v xml:space="preserve">T Natarajan </v>
       </c>
       <c r="B160">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E160">
         <v>0</v>
@@ -3590,16 +3590,16 @@
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v xml:space="preserve">Dhawal Kulkarni </v>
+        <v xml:space="preserve">Tabraiz Shamsi </v>
       </c>
       <c r="B161">
         <v>1</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D161">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E161">
         <v>0</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v xml:space="preserve">Anuj Rawat </v>
+        <v xml:space="preserve">Ben Stokes </v>
       </c>
       <c r="B162">
         <v>1</v>
@@ -3619,7 +3619,7 @@
         <v>0</v>
       </c>
       <c r="D162">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E162">
         <v>0</v>

</xml_diff>